<commit_message>
add new ferrite bead
</commit_message>
<xml_diff>
--- a/pcb/order-list/BOM.xlsx
+++ b/pcb/order-list/BOM.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tdt4295\tdt4295-grafikk\pcb\order-list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Emblas Data\Documents\Skole\Semester\7\tdt4295-grafikk\pcb\order-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6DE6DE-9569-4AAB-BD75-B37E672580C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{054738BD-EEFE-4B42-A841-E5EEC52CD301}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="11625"/>
   </bookViews>
   <sheets>
     <sheet name="tdt4295_bom_" sheetId="2" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <definedNames>
     <definedName name="EksterneData_1" localSheetId="0" hidden="1">tdt4295_bom_!$A$1:$V$67</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,15 +37,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{90FC7396-20C8-4E52-835D-D75E5699BB16}" keepAlive="1" name="Spørring - tdt4295_bom_" description="Tilkobling til spørringen tdt4295_bom_ i arbeidsboken." type="5" refreshedVersion="7" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="Spørring - tdt4295_bom_" description="Tilkobling til spørringen tdt4295_bom_ i arbeidsboken." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=tdt4295_bom_;Extended Properties=&quot;&quot;" command="SELECT * FROM [tdt4295_bom_]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="407">
   <si>
     <t>Component</t>
   </si>
@@ -1261,16 +1260,30 @@
   </si>
   <si>
     <t>Quantity ordered</t>
+  </si>
+  <si>
+    <t>https://no.farnell.com/wurth-elektronik/74279201/ferrite-bead-0-15-ohm-0-5a-0805/dp/1635708</t>
+  </si>
+  <si>
+    <t>32Ohm@100MHz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1293,14 +1306,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
@@ -1381,7 +1397,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="EksterneData_1" connectionId="1" xr16:uid="{EE064911-5F14-4369-BC03-9265C1AEE4B7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="EksterneData_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="23">
     <queryTableFields count="22">
       <queryTableField id="1" name="Component" tableColumnId="1"/>
@@ -1412,31 +1428,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1CE2E346-0BE2-4256-B23A-EAD227A5EBE9}" name="tdt4295_bom_" displayName="tdt4295_bom_" ref="A1:V67" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:V67" xr:uid="{1CE2E346-0BE2-4256-B23A-EAD227A5EBE9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tdt4295_bom_" displayName="tdt4295_bom_" ref="A1:V67" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:V67"/>
   <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{6160EEFD-0281-4A6D-A766-AB9C95B84119}" uniqueName="1" name="Component" queryTableFieldId="1" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{A55C869E-CDA6-4944-82DF-517460EF81DB}" uniqueName="2" name="Description" queryTableFieldId="2" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{4E6DF28E-8942-4A69-92C5-38B41091EBF7}" uniqueName="3" name="Part" queryTableFieldId="3" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{4F208CED-4CB8-4767-8FFF-5F4198149EB5}" uniqueName="4" name="References" queryTableFieldId="4" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{EB3407AB-9EE1-4663-9EC7-59E6A0459C11}" uniqueName="5" name="Value" queryTableFieldId="5" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{9285D943-805A-4202-90EF-0AD181787261}" uniqueName="6" name="Footprint" queryTableFieldId="6" dataDxfId="15"/>
-    <tableColumn id="22" xr3:uid="{65EE4263-CB0A-46B9-891B-8B789990BAD7}" uniqueName="22" name="Quantity ordered" queryTableFieldId="22" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{A579B508-62DB-4F23-91E0-3C1B2452D783}" uniqueName="7" name="Quantity Per PCB" queryTableFieldId="7"/>
-    <tableColumn id="8" xr3:uid="{9D9C5886-53B6-4C1D-A82B-395A5B721E5C}" uniqueName="8" name="Datasheet" queryTableFieldId="8" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{E64ED41D-6E61-490A-B383-1B770706B187}" uniqueName="9" name="Digi-Key_PN" queryTableFieldId="9" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{FD5097B3-9C02-41BD-8893-DB405E11DB07}" uniqueName="10" name="DK_Datasheet_Link" queryTableFieldId="10" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{AA5E82F7-55DA-418D-8586-75104D177A6D}" uniqueName="11" name="DK_Detail_Page" queryTableFieldId="11" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{248D799A-9AA6-4E15-ADCB-98509633DCBE}" uniqueName="12" name="Component name" queryTableFieldId="12" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{2E172604-5F1D-4CF9-94AD-E9668CC584BC}" uniqueName="13" name="MANUFACTURER" queryTableFieldId="13" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{D1E1411A-1027-4B30-AE94-14C27FCDE017}" uniqueName="14" name="Category" queryTableFieldId="14" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{4B5E8EE6-2F7B-4F3D-8B49-DA75AFB82E69}" uniqueName="15" name="Status" queryTableFieldId="15" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{FD0F0B2A-C0E5-4225-9D75-26D47CA4382E}" uniqueName="16" name="Family" queryTableFieldId="16" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{B9670231-1C11-4D7F-A4A5-5256ED4790CC}" uniqueName="17" name="MPN" queryTableFieldId="17" dataDxfId="5"/>
-    <tableColumn id="18" xr3:uid="{34B81056-38FF-4501-83FD-97F4AAC39B9C}" uniqueName="18" name="Manufacturer.1" queryTableFieldId="18" dataDxfId="4"/>
-    <tableColumn id="19" xr3:uid="{2DBACCF1-5678-40C7-87D9-063DEB776930}" uniqueName="19" name="MAXIMUM_PACKAGE_HEIGHT" queryTableFieldId="19" dataDxfId="3"/>
-    <tableColumn id="20" xr3:uid="{450FAC44-12A5-4852-93F6-A870EC2D395E}" uniqueName="20" name="STANDARD" queryTableFieldId="20" dataDxfId="2"/>
-    <tableColumn id="21" xr3:uid="{CEAEF6B5-5F84-4B5A-B134-C45897CE4072}" uniqueName="21" name="PARTREV" queryTableFieldId="21" dataDxfId="1"/>
+    <tableColumn id="1" uniqueName="1" name="Component" queryTableFieldId="1" dataDxfId="20"/>
+    <tableColumn id="2" uniqueName="2" name="Description" queryTableFieldId="2" dataDxfId="19"/>
+    <tableColumn id="3" uniqueName="3" name="Part" queryTableFieldId="3" dataDxfId="18"/>
+    <tableColumn id="4" uniqueName="4" name="References" queryTableFieldId="4" dataDxfId="17"/>
+    <tableColumn id="5" uniqueName="5" name="Value" queryTableFieldId="5" dataDxfId="16"/>
+    <tableColumn id="6" uniqueName="6" name="Footprint" queryTableFieldId="6" dataDxfId="15"/>
+    <tableColumn id="22" uniqueName="22" name="Quantity ordered" queryTableFieldId="22" dataDxfId="14"/>
+    <tableColumn id="7" uniqueName="7" name="Quantity Per PCB" queryTableFieldId="7"/>
+    <tableColumn id="8" uniqueName="8" name="Datasheet" queryTableFieldId="8" dataDxfId="13"/>
+    <tableColumn id="9" uniqueName="9" name="Digi-Key_PN" queryTableFieldId="9" dataDxfId="12"/>
+    <tableColumn id="10" uniqueName="10" name="DK_Datasheet_Link" queryTableFieldId="10" dataDxfId="11"/>
+    <tableColumn id="11" uniqueName="11" name="DK_Detail_Page" queryTableFieldId="11" dataDxfId="10"/>
+    <tableColumn id="12" uniqueName="12" name="Component name" queryTableFieldId="12" dataDxfId="9"/>
+    <tableColumn id="13" uniqueName="13" name="MANUFACTURER" queryTableFieldId="13" dataDxfId="8"/>
+    <tableColumn id="14" uniqueName="14" name="Category" queryTableFieldId="14" dataDxfId="7"/>
+    <tableColumn id="15" uniqueName="15" name="Status" queryTableFieldId="15" dataDxfId="6"/>
+    <tableColumn id="16" uniqueName="16" name="Family" queryTableFieldId="16" dataDxfId="5"/>
+    <tableColumn id="17" uniqueName="17" name="MPN" queryTableFieldId="17" dataDxfId="4"/>
+    <tableColumn id="18" uniqueName="18" name="Manufacturer.1" queryTableFieldId="18" dataDxfId="3"/>
+    <tableColumn id="19" uniqueName="19" name="MAXIMUM_PACKAGE_HEIGHT" queryTableFieldId="19" dataDxfId="2"/>
+    <tableColumn id="20" uniqueName="20" name="STANDARD" queryTableFieldId="20" dataDxfId="1"/>
+    <tableColumn id="21" uniqueName="21" name="PARTREV" queryTableFieldId="21" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1738,39 +1754,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB15A8B6-A704-45F4-B851-DA24C339784A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I55" sqref="I54:I55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.54296875" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" customWidth="1"/>
-    <col min="4" max="4" width="35.6328125" customWidth="1"/>
-    <col min="5" max="5" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.90625" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="80.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="41.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="80.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="38.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.90625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="28.6328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1838,7 +1854,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -1906,7 +1922,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>33</v>
       </c>
@@ -1974,7 +1990,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -2042,7 +2058,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
@@ -2110,7 +2126,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
@@ -2178,7 +2194,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>60</v>
       </c>
@@ -2246,7 +2262,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>66</v>
       </c>
@@ -2314,7 +2330,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>73</v>
       </c>
@@ -2382,7 +2398,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>81</v>
       </c>
@@ -2450,7 +2466,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>86</v>
       </c>
@@ -2518,7 +2534,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>92</v>
       </c>
@@ -2586,7 +2602,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>98</v>
       </c>
@@ -2654,7 +2670,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>106</v>
       </c>
@@ -2722,7 +2738,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>114</v>
       </c>
@@ -2790,7 +2806,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>123</v>
       </c>
@@ -2858,7 +2874,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>132</v>
       </c>
@@ -2926,7 +2942,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>141</v>
       </c>
@@ -2994,7 +3010,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>150</v>
       </c>
@@ -3062,7 +3078,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>159</v>
       </c>
@@ -3130,7 +3146,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>168</v>
       </c>
@@ -3198,7 +3214,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>177</v>
       </c>
@@ -3266,7 +3282,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>183</v>
       </c>
@@ -3334,7 +3350,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>195</v>
       </c>
@@ -3402,7 +3418,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>204</v>
       </c>
@@ -3470,7 +3486,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>213</v>
       </c>
@@ -3538,7 +3554,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>221</v>
       </c>
@@ -3606,7 +3622,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>228</v>
       </c>
@@ -3674,7 +3690,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>235</v>
       </c>
@@ -3742,7 +3758,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>241</v>
       </c>
@@ -3810,7 +3826,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>248</v>
       </c>
@@ -3878,7 +3894,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>255</v>
       </c>
@@ -3946,7 +3962,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>262</v>
       </c>
@@ -4012,7 +4028,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>268</v>
       </c>
@@ -4080,7 +4096,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>276</v>
       </c>
@@ -4148,7 +4164,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>282</v>
       </c>
@@ -4216,7 +4232,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>288</v>
       </c>
@@ -4284,7 +4300,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>294</v>
       </c>
@@ -4352,7 +4368,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>301</v>
       </c>
@@ -4420,7 +4436,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>307</v>
       </c>
@@ -4488,7 +4504,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>313</v>
       </c>
@@ -4556,7 +4572,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>319</v>
       </c>
@@ -4624,7 +4640,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>330</v>
       </c>
@@ -4692,7 +4708,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>341</v>
       </c>
@@ -4760,7 +4776,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>347</v>
       </c>
@@ -4826,7 +4842,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>351</v>
       </c>
@@ -4892,7 +4908,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>354</v>
       </c>
@@ -4958,7 +4974,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>362</v>
       </c>
@@ -5024,7 +5040,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>367</v>
       </c>
@@ -5090,7 +5106,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>372</v>
       </c>
@@ -5156,7 +5172,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>377</v>
       </c>
@@ -5222,7 +5238,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>32</v>
       </c>
@@ -5230,18 +5246,21 @@
         <v>32</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>32</v>
+        <v>109</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>406</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>32</v>
+        <v>230</v>
       </c>
       <c r="G52" s="1"/>
+      <c r="H52">
+        <v>1</v>
+      </c>
       <c r="I52" s="1" t="s">
         <v>32</v>
       </c>
@@ -5252,7 +5271,7 @@
         <v>32</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>32</v>
+        <v>405</v>
       </c>
       <c r="M52" s="1" t="s">
         <v>32</v>
@@ -5285,7 +5304,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>32</v>
       </c>
@@ -5348,7 +5367,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>32</v>
       </c>
@@ -5411,7 +5430,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>32</v>
       </c>
@@ -5474,7 +5493,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>32</v>
       </c>
@@ -5537,7 +5556,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>386</v>
       </c>
@@ -5600,7 +5619,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>387</v>
       </c>
@@ -5663,7 +5682,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>389</v>
       </c>
@@ -5726,7 +5745,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>390</v>
       </c>
@@ -5789,7 +5808,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>391</v>
       </c>
@@ -5852,7 +5871,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>392</v>
       </c>
@@ -5915,7 +5934,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>393</v>
       </c>
@@ -5978,7 +5997,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>394</v>
       </c>
@@ -6041,7 +6060,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>396</v>
       </c>
@@ -6104,7 +6123,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>398</v>
       </c>
@@ -6167,7 +6186,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>400</v>
       </c>
@@ -6231,20 +6250,23 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E52" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6788AA5-5B72-4C5A-9326-621DFA2D630A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>